<commit_message>
Some tests regarding the calculation and tagging of dates.
</commit_message>
<xml_diff>
--- a/ExcelLifeBook/Twainsoft.Blog.Examples.ExcelLifeBook/Twainsoft.Blog.Examples.ExcelLifeBook.xlsx
+++ b/ExcelLifeBook/Twainsoft.Blog.Examples.ExcelLifeBook/Twainsoft.Blog.Examples.ExcelLifeBook.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13350" windowHeight="10470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22305" windowHeight="12105"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -339,7 +339,9 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>